<commit_message>
Update to R 4.3 and packages
</commit_message>
<xml_diff>
--- a/data-raw/Example_input_file.xlsx
+++ b/data-raw/Example_input_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud\Nature Analytics web apps\Packages and modules\fishSimTools\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6CB7F0-E96A-4F39-8848-B587CBD61376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9885F6D-5D28-4B4D-A986-07B9EB23E269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3744" yWindow="2484" windowWidth="19164" windowHeight="8964" tabRatio="951" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="951" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="13" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="120">
   <si>
     <t>speciesName</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Steep</t>
   </si>
   <si>
-    <t>inHermaph</t>
-  </si>
-  <si>
     <t>H50</t>
   </si>
   <si>
@@ -192,18 +189,6 @@
     <t>proj_bag_row</t>
   </si>
   <si>
-    <t>Area_1_1</t>
-  </si>
-  <si>
-    <t>Area_1_2</t>
-  </si>
-  <si>
-    <t>Area_2_1</t>
-  </si>
-  <si>
-    <t>Area_2_2</t>
-  </si>
-  <si>
     <t>title</t>
   </si>
   <si>
@@ -285,9 +270,6 @@
     <t>Bag_pars</t>
   </si>
   <si>
-    <t>Bag limits for each area. A value of -99 will produce on bag limit for the area. A row represents a scenario. Enter 1 value in each column for the number of areas in your model.</t>
-  </si>
-  <si>
     <t>1,1</t>
   </si>
   <si>
@@ -312,9 +294,6 @@
     <t>Status quo is the short label that is used in the plotting functions,this does not have to be unique it is simply a plot label</t>
   </si>
   <si>
-    <t xml:space="preserve"> proFisheryVul_list</t>
-  </si>
-  <si>
     <t>DO NOT CHANGE THE NAMES OF HEADERS</t>
   </si>
   <si>
@@ -355,6 +334,78 @@
   </si>
   <si>
     <t>Tmax</t>
+  </si>
+  <si>
+    <t>Stochastic_base</t>
+  </si>
+  <si>
+    <t>Title - a string</t>
+  </si>
+  <si>
+    <t>Two values separated by a comma, min and max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One value, a row number corresponding to Sel_uncertainty_pars. Corresponding row contains sel params  in 'fill by row R format'. See info for Sel_uncertainty_pars </t>
+  </si>
+  <si>
+    <t>proFisheryVul_list</t>
+  </si>
+  <si>
+    <t>Logical. Indicates whether values generated for corresponding historical object should be applied to projection object as well</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A value for each area separated by a comma corresponding to Sel_uncertainty_pars. Corresponding rows contains sel params  in 'fill by row R format'. See info for Sel_uncertainty_pars </t>
+  </si>
+  <si>
+    <t>Effort_pars</t>
+  </si>
+  <si>
+    <t>Row contains effort multiplier for each area.</t>
+  </si>
+  <si>
+    <t>These values will fill maxtrices of n cols equal to number of areas and n rows equal years</t>
+  </si>
+  <si>
+    <t>If all areas and years are to contain the same value, 1 value can be entered which will be repeated in populating the effort matrix</t>
+  </si>
+  <si>
+    <t>Bag limits for each area. A value of -99 will produce no bag limit for the area. A row represents a scenario. Enter 1 value in each column for the number of areas in your model.</t>
+  </si>
+  <si>
+    <t>Movement_pars</t>
+  </si>
+  <si>
+    <t>Used to create a matrix of nrow = area by ncol = area</t>
+  </si>
+  <si>
+    <t>For example, values as follows for a 2 by 2 matrix</t>
+  </si>
+  <si>
+    <t>Each column should sum to 1. Each column is j --&gt; i. In j, moving to i</t>
+  </si>
+  <si>
+    <t>The example:</t>
+  </si>
+  <si>
+    <t>80% staying in area 1, 20% moving to area 2</t>
+  </si>
+  <si>
+    <t>30% moving from area 2 to area 1, 70% staying in area 2</t>
+  </si>
+  <si>
+    <t>Area_in_1_going_to_1</t>
+  </si>
+  <si>
+    <t>Area_in_1_going_to_2</t>
+  </si>
+  <si>
+    <t>Area_in_2_going_to_1</t>
+  </si>
+  <si>
+    <t>Area_in_2_going_to_2</t>
+  </si>
+  <si>
+    <t>isHermaph</t>
   </si>
 </sst>
 </file>
@@ -694,132 +745,408 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7BE5C2-CEE1-4216-80DC-AAA61EF36988}">
-  <dimension ref="B3:E33"/>
+  <dimension ref="B3:E70"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29:E29"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="21.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>0.8</v>
+      </c>
+      <c r="C15">
+        <v>0.2</v>
+      </c>
+      <c r="D15">
+        <v>0.3</v>
+      </c>
+      <c r="E15">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>0.8</v>
+      </c>
+      <c r="C17">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>0.2</v>
+      </c>
+      <c r="C18">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B29" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B32" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B7" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B25" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <v>20</v>
+      </c>
+      <c r="C36">
+        <v>30</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <v>20</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B39">
+        <v>30</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B42" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B29">
-        <v>20</v>
-      </c>
-      <c r="C29">
-        <v>30</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B31">
-        <v>20</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B32">
-        <v>30</v>
-      </c>
-      <c r="C32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
+      <c r="C46" t="s">
         <v>98</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>49</v>
+      </c>
+      <c r="C48" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>57</v>
+      </c>
+      <c r="C52" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>50</v>
+      </c>
+      <c r="C54" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>100</v>
+      </c>
+      <c r="C56" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>59</v>
+      </c>
+      <c r="C57" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
+        <v>60</v>
+      </c>
+      <c r="C58" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>83</v>
+      </c>
+      <c r="C59" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>61</v>
+      </c>
+      <c r="C60" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
+        <v>62</v>
+      </c>
+      <c r="C61" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>84</v>
+      </c>
+      <c r="C62" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>63</v>
+      </c>
+      <c r="C63" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B68" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -904,7 +1231,7 @@
   <dimension ref="A1:AX3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1186,36 +1513,36 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
         <v>40</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
         <v>41</v>
       </c>
-      <c r="E1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>42</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>43</v>
-      </c>
-      <c r="H1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1230,7 +1557,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -1245,8 +1572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BF90675-A8BE-4A28-87BD-FF30F3F0ACD5}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1273,7 +1600,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1291,7 +1618,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>5</v>
@@ -1312,33 +1639,33 @@
         <v>10</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="P1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="R1" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="S1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="T1" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
         <v>27</v>
-      </c>
-      <c r="B2" t="s">
-        <v>28</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -1359,10 +1686,10 @@
         <v>0.25</v>
       </c>
       <c r="I2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" t="s">
         <v>29</v>
-      </c>
-      <c r="J2" t="s">
-        <v>30</v>
       </c>
       <c r="K2">
         <v>0.01</v>
@@ -1398,7 +1725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DCC4F28-3F04-4582-AF80-CDD047BEA0A1}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -1418,39 +1745,39 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" t="s">
-        <v>19</v>
-      </c>
       <c r="J1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2">
         <v>13</v>
@@ -1474,7 +1801,7 @@
         <v>0.5</v>
       </c>
       <c r="I2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -1506,42 +1833,42 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>23</v>
-      </c>
-      <c r="G1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1559,8 +1886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE4C6808-4753-4C78-9BA1-C1E56B942589}">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1580,10 +1907,10 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1595,7 +1922,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -1604,51 +1931,51 @@
         <v>10</v>
       </c>
       <c r="I1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N1" t="s">
+        <v>100</v>
+      </c>
+      <c r="O1" t="s">
+        <v>59</v>
+      </c>
+      <c r="P1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>83</v>
+      </c>
+      <c r="R1" t="s">
+        <v>61</v>
+      </c>
+      <c r="S1" t="s">
         <v>62</v>
       </c>
-      <c r="K1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" t="s">
-        <v>55</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="T1" t="s">
+        <v>84</v>
+      </c>
+      <c r="U1" t="s">
         <v>63</v>
-      </c>
-      <c r="N1" t="s">
-        <v>88</v>
-      </c>
-      <c r="O1" t="s">
-        <v>64</v>
-      </c>
-      <c r="P1" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>90</v>
-      </c>
-      <c r="R1" t="s">
-        <v>66</v>
-      </c>
-      <c r="S1" t="s">
-        <v>67</v>
-      </c>
-      <c r="T1" t="s">
-        <v>91</v>
-      </c>
-      <c r="U1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1677,36 +2004,36 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" t="s">
-        <v>26</v>
-      </c>
       <c r="D1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B2">
         <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1715,10 +2042,10 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1756,23 +2083,29 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.77734375" customWidth="1"/>
+    <col min="2" max="2" width="24.77734375" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>115</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>116</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>117</v>
       </c>
       <c r="D1" t="s">
-        <v>51</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>